<commit_message>
updated xls wall motivation
</commit_message>
<xml_diff>
--- a/workspace/Algorithms.xlsx
+++ b/workspace/Algorithms.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="11140" yWindow="380" windowWidth="22980" windowHeight="27880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Wall-Motivation-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wall-Motivation-2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
@@ -20,118 +21,221 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+  <si>
+    <t>Simple Immunological Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radial Bias Function</t>
+  </si>
+  <si>
+    <t>Reactive Tabu Search</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genetic Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genetic Programming</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evolution Strategies</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Differential Evolution</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene Expression Programming</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning Classifier System</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clonal Selection Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Negative Selection Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immune Network Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dendritic Cell Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-Organizing Map</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hopfield Network</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kingdom</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algorithm (to describe)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immune</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swarm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physical</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probabilistic</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neural</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bees Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cultural Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-Cell Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backup Algorithms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross-Entropy Method</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantum Annealing</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adaptive Simulated Annealing</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max-Min Ant System</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bacterial Foraging Optimization Algorithm</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t>Simulated Annealing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Adaptive Simulated Annealing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Mementic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Extremal Optimization</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Cultural Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Ant System</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Must Have Algorithms</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Easy Algorithms</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cellular Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crowding Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Island Population Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B-Cell Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Artificial Immune Recognition System</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Neural</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Perceptron</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Back Propagation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Hopfield</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Self Organization Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Learning Vector Quantization</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Linkage Learning Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Deterministic Crowding Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Vector Evaluated Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Guided Local Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Pareto Archived Evolution Strategy</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Bees Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Milestone</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Population-Based Incremental Learning</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Particle Swarm Optimization</t>
@@ -159,143 +263,104 @@
   </si>
   <si>
     <t>Univariate Marginal Distribution Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Ant Colony System</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>#</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Kingdom</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Stochastic</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Evolutionary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Immune</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Evolutionary</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Physical</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Swarm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Probabilistic</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Evolutionary Programming</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Grammatical Evolution</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>HALF WAY!</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Messy Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Random Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Adaptive Random Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Hill Climbing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Iterated Local Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Variable Neighborhood Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Scatter Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Tabu Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reactive Tabu Search</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genetic Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genetic Programming</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Evolution Strategies</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Differential Evolution</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene Expression Programming</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Learning Classifier System</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Clonal Selection Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Negative Selection Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Immune Network Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dendritic Cell Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -418,22 +483,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -767,8 +834,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D40"/>
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -781,16 +848,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -801,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -813,10 +880,10 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -825,10 +892,10 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -837,10 +904,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -849,10 +916,10 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -861,10 +928,10 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -873,10 +940,10 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -885,10 +952,10 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -897,10 +964,10 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -909,10 +976,10 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -923,10 +990,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -935,10 +1002,10 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -947,10 +1014,10 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -959,10 +1026,10 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -971,10 +1038,10 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -983,10 +1050,10 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -995,10 +1062,10 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1007,10 +1074,10 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1019,10 +1086,10 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1031,10 +1098,10 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1045,10 +1112,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1057,10 +1124,10 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1069,10 +1136,10 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1081,10 +1148,10 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1093,13 +1160,13 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1108,10 +1175,10 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1120,10 +1187,10 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1132,10 +1199,10 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1144,10 +1211,10 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1156,10 +1223,10 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1170,10 +1237,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1182,10 +1249,10 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1194,10 +1261,10 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1206,10 +1273,10 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1218,10 +1285,10 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1230,10 +1297,10 @@
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1242,10 +1309,10 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1254,10 +1321,10 @@
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1266,10 +1333,10 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1278,10 +1345,10 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1292,10 +1359,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1304,10 +1371,10 @@
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1316,10 +1383,10 @@
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1328,10 +1395,10 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1340,10 +1407,10 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1352,10 +1419,10 @@
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1364,10 +1431,10 @@
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1376,10 +1443,10 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1388,10 +1455,10 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1400,14 +1467,14 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1421,90 +1488,207 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="3"/>
+      <c r="B11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>